<commit_message>
added week 2 pbp
</commit_message>
<xml_diff>
--- a/elo change.xlsx
+++ b/elo change.xlsx
@@ -59,8 +59,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
-    <numFmt numFmtId="165" formatCode="0.000"/>
-    <numFmt numFmtId="166" formatCode="0.0"/>
+    <numFmt numFmtId="164" formatCode="0.000"/>
+    <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -102,9 +102,9 @@
   <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -407,7 +407,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E12"/>
+  <dimension ref="A1:J12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B7" sqref="B7"/>
@@ -418,7 +418,7 @@
     <col min="1" max="1" width="9.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>9</v>
       </c>
@@ -429,48 +429,64 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
       <c r="B2">
-        <v>1483.75</v>
+        <v>1507.827</v>
       </c>
       <c r="C2" s="3">
         <f>(B2-1500)/25</f>
-        <v>-0.65</v>
+        <v>0.31307999999999991</v>
       </c>
       <c r="D2" s="3">
         <f>C2-B12/25</f>
-        <v>0.43693225155216375</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+        <v>5.5447905040224066E-2</v>
+      </c>
+      <c r="F2" s="3">
+        <f>B2-B12</f>
+        <v>1501.3861976260057</v>
+      </c>
+      <c r="I2">
+        <v>1510.923</v>
+      </c>
+      <c r="J2">
+        <v>1507.827</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>0</v>
       </c>
       <c r="B3">
-        <v>1535</v>
+        <v>1464.298</v>
       </c>
       <c r="C3" s="3">
         <f>(B3-1500)/25</f>
-        <v>1.4</v>
+        <v>-1.42808</v>
       </c>
       <c r="D3" s="3">
         <f>C3+B12/25</f>
-        <v>0.31306774844783614</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+        <v>-1.1704479050402241</v>
+      </c>
+      <c r="I3">
+        <v>1509.452</v>
+      </c>
+      <c r="J3">
+        <v>1464.298</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>2</v>
       </c>
       <c r="B5" s="1">
         <f>1/(1+10^(-(B3-B2+65)/400))</f>
-        <v>0.66132149251579797</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+        <v>0.53085997751059999</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -478,54 +494,54 @@
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>5</v>
       </c>
       <c r="B7">
-        <v>-6</v>
+        <v>1</v>
       </c>
       <c r="E7">
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>3</v>
       </c>
       <c r="B8" s="3">
         <f>(IF(B7&lt;0,-B5,1-B5))*B6</f>
-        <v>-13.226429850315959</v>
+        <v>9.3828004497880002</v>
       </c>
       <c r="E8">
         <v>-3</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>6</v>
       </c>
       <c r="B9" s="3">
         <f>LN(ABS(B7)+1)</f>
-        <v>1.9459101490553132</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+        <v>0.69314718055994529</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>7</v>
       </c>
       <c r="B10" s="2">
         <f>2.2/(2.2+(IF(B7&gt;0,1/1000,-1/1000)*(B3-B2+65)))</f>
-        <v>1.0557888422315536</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+        <v>0.99033478267328268</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>8</v>
       </c>
       <c r="B12" s="4">
         <f>B8*B9*B10</f>
-        <v>-27.173306288804095</v>
+        <v>6.440802373994396</v>
       </c>
     </row>
   </sheetData>

</xml_diff>